<commit_message>
grinnel doc checkpoint + frp background checkpoint
</commit_message>
<xml_diff>
--- a/grinnell_docs/nsf20-medium-fet-budget-osera.xlsx
+++ b/grinnell_docs/nsf20-medium-fet-budget-osera.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/osera/Repositories/medium-2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/osera/Repositories/frmp-nsf-medium/grinnell_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490B498E-9D66-D944-9CA5-AC19115AFB2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0666BCE9-4D56-F444-BF7F-D276DBC36AD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -23,6 +23,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -152,7 +153,7 @@
     <t>I. Indirect Costs</t>
   </si>
   <si>
-    <t>PI and hourly wages (62%)</t>
+    <t>PI and hourly wages (65%)</t>
   </si>
 </sst>
 </file>
@@ -558,7 +559,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -619,24 +620,24 @@
         <v>10</v>
       </c>
       <c r="B3" s="3">
-        <f>23838.78*I12</f>
-        <v>11919.39</v>
+        <f>24061*I12</f>
+        <v>24061</v>
       </c>
       <c r="C3" s="3">
-        <f>24776.16*I12</f>
-        <v>12388.08</v>
+        <f>24782.83*I12</f>
+        <v>24782.83</v>
       </c>
       <c r="D3" s="3">
-        <f>25519.45*I12</f>
-        <v>12759.725</v>
+        <f>25526.31*I12</f>
+        <v>25526.31</v>
       </c>
       <c r="E3" s="3">
-        <f>26285.03*I12</f>
-        <v>13142.514999999999</v>
+        <f>26292.1*I12</f>
+        <v>26292.1</v>
       </c>
       <c r="F3" s="4">
         <f>SUM(B3:E3)</f>
-        <v>50209.71</v>
+        <v>100662.23999999999</v>
       </c>
       <c r="H3" t="s">
         <v>11</v>
@@ -780,23 +781,23 @@
       </c>
       <c r="B9" s="3">
         <f>I7*B3</f>
-        <v>2103.7723349999997</v>
+        <v>4246.7664999999997</v>
       </c>
       <c r="C9" s="3">
         <f>I7*C3</f>
-        <v>2186.4961199999998</v>
+        <v>4374.1694950000001</v>
       </c>
       <c r="D9" s="3">
         <f>I7*D3</f>
-        <v>2252.0914625</v>
+        <v>4505.3937150000002</v>
       </c>
       <c r="E9" s="3">
         <f>I7*E3</f>
-        <v>2319.6538974999999</v>
+        <v>4640.5556499999993</v>
       </c>
       <c r="F9" s="4">
         <f>SUM(B9:E9)</f>
-        <v>8862.0138150000002</v>
+        <v>17766.88536</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>25</v>
@@ -876,7 +877,7 @@
         <v>31</v>
       </c>
       <c r="I12" s="13">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1063,23 +1064,23 @@
       </c>
       <c r="B23" s="3">
         <f>(B3+B5+B7)*I10</f>
-        <v>10368.4035</v>
+        <v>18260.45</v>
       </c>
       <c r="C23" s="3">
         <f>(C3+C5+C7)*I10</f>
-        <v>10673.052000000001</v>
+        <v>18729.639500000001</v>
       </c>
       <c r="D23" s="3">
         <f>(D3+D5+D7)*I10</f>
-        <v>10914.62125</v>
+        <v>19212.9015</v>
       </c>
       <c r="E23" s="3">
         <f>(E3+E5+E7)*I10</f>
-        <v>11163.43475</v>
+        <v>19710.665000000001</v>
       </c>
       <c r="F23" s="4">
         <f>SUM(B23:E23)</f>
-        <v>43119.511500000008</v>
+        <v>75913.656000000003</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1095,23 +1096,23 @@
       </c>
       <c r="B25" s="4">
         <f>SUM(B2:B24)</f>
-        <v>53403.565835000001</v>
+        <v>75580.216499999995</v>
       </c>
       <c r="C25" s="4">
         <f t="shared" ref="C25:E25" si="0">SUM(C2:C24)</f>
-        <v>57759.628120000001</v>
+        <v>80398.638995000001</v>
       </c>
       <c r="D25" s="4">
         <f t="shared" si="0"/>
-        <v>52438.437712500003</v>
+        <v>75756.605214999989</v>
       </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>59137.6036475</v>
+        <v>83155.320650000009</v>
       </c>
       <c r="F25" s="8">
         <f>SUM(F2:F24)</f>
-        <v>222739.235315</v>
+        <v>314890.78136000002</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>